<commit_message>
proper functioning data extraction
</commit_message>
<xml_diff>
--- a/all_tables.xlsx
+++ b/all_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Backup\Web Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875163B2-3259-4E47-A5F6-D2FB0AC0AD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CD264D-2377-494F-A7AA-482BB72335D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
-  <si>
-    <t>Tender ID- 200654View BOQ/Item Details</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
+  <si>
+    <t>Tender ID- 200717View BOQ/Item Details</t>
   </si>
   <si>
     <t>Organization Name</t>
@@ -43,13 +43,13 @@
     <t>Sub Department</t>
   </si>
   <si>
-    <t>S.C. Electrical Sub Division No. 2</t>
+    <t>S.C. Electrical Sub Division No. 3</t>
   </si>
   <si>
     <t>IFB/Tender Notice No</t>
   </si>
   <si>
-    <t>05/02 OF 2025/2026</t>
+    <t>05/04 OF 2025/2026</t>
   </si>
   <si>
     <t>Tender Type</t>
@@ -61,7 +61,7 @@
     <t>Tender title/Name Of Project</t>
   </si>
   <si>
-    <t>AMC of Pumps for Utility Block &amp; Swarnim Sankul 1&amp;2,new Sachivalaya, Gandhinagar.(For One Year)(2nd Attempt)</t>
+    <t>PROVIDING STREET LIGHT POLES AT VARIOUS PLACES UNDER STREET LIGHT SECTION,GANDHINAGAR</t>
   </si>
   <si>
     <t>Description of Material/Name of Work</t>
@@ -82,7 +82,7 @@
     <t>Product Category</t>
   </si>
   <si>
-    <t>Electrical and Maintenance Works</t>
+    <t>Electrical</t>
   </si>
   <si>
     <t>Tender Category</t>
@@ -94,7 +94,7 @@
     <t>Estimated Cost Value</t>
   </si>
   <si>
-    <t>533208.03 INR.  (Five lacs Thirty Three Thousand Two hundred Eight Point Zero Three Only)</t>
+    <t>306982.43 INR.  (Three lacs Zero Six Thousand Nine hundred Eighty Two Point Four  Three Only)</t>
   </si>
   <si>
     <t>Is ECV Visible to Supplier?</t>
@@ -118,7 +118,7 @@
     <t>Period of Completion/Delivery Period</t>
   </si>
   <si>
-    <t>1  Years</t>
+    <t>20  Days</t>
   </si>
   <si>
     <t>Procurement Type</t>
@@ -142,7 +142,7 @@
     <t>Bid Document Download Start Date</t>
   </si>
   <si>
-    <t>02-07-2025 11:00</t>
+    <t>02-07-2025 12:15</t>
   </si>
   <si>
     <t>Bid document download End Date</t>
@@ -163,7 +163,8 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Demand Draft Tender fee and E.M.D. in FDR form (not Less than 180 days) / Exemption Certificate / Demand Draft shall be submitted in electronic format only through online (by scanning) while uploading the bid. This submission shall mean that E.M.D. &amp; tender fee are received for purpose of opening the bid. Accordingly offer of those shall be opened whose E.M.D. and tender fee is received electronically. However for the purpose of realization of D.D. bidder shall send the D.D. in original through R.P.A.D. / Speed Post / Courier so as to reach to Dy. Executive Engineer, Sachivalaya Complex Electrical Sub Division No 2, Gandhinagar within 7 days from the date of tender opening. Penaltative action for not submitting D.D. in original to Deputy Executive Engineer by bidder shall be initiated. However Exemption Certificate shall have to be submitted electronically through online. If the contractor does not remit the tender fee &amp; the earnest money within the specified time his registration will be held in abeyance for one year &amp; his tendering code will be cancelled for one year. Any documents in supporting of tender bid shall be submitted in electronic format only through online (by scanning etc.) and hard copy will not be accepted separately. (R. &amp; B. Circular No: PRC-102008-5-S, dated 18-01-2008 &amp; R. &amp; B. D.G.R.No: Parach-102008-5-C (Partfile), dated 27-11-2008). All bidders are requested to verify all uploaded documents before proceed for final submission. If any document is Corrupted / Not uploaded properly during the uploading may not be opened while evaluation. Which may lead to disqualification therefore it is recommended to view document after uploading in the tender.</t>
+    <t>Demand Draft Tender fee and E.M.D. in FDR form (not Less than 180 days) / Demand Drfat / Exemption Certificate shall be submitted in electronic format only through online (by scanning) while uploading the bid. This submission shall mean that E.M.D. &amp; tender fee are received for purpose of opening the bid. Accordingly offer of those shall be opened whose E.M.D. and tender fee is received electronically. However for the purpose of realization of D.D. bidder shall send the D.D. in original through R.P.A.D. so as to reach to Dy. Executive Engineer, Sachivalaya Complex Electrical Sub Division No. 3, Gandhinagar within 7 days from the date of tender Opening. Penaltative action for not submitting D.D. in original to Executive Engineer by bidder shall be initiated. D.D. for Exemption Certificate is not necessary. However Exemption Certificate shall have to be submitted electronically through online. If the contractor does not remit the tender fee &amp; the earnest money within the specified time his registration will be held in abeyance for one year &amp; his tendering code will be cancelled for one year. Any documents in supporting of tender bid shall be submitted in electronic format only through online (by scanning etc.) and hard copy will not be accepted separately. (R. &amp; B. Circular No: PRC-102008-5-S, dated 18-01-2008 &amp; R. &amp; B. D.G.R.No: Parach-102008-5-C (Partfile), dated 27-11-2008). Note:- Only Tender Fee and E.M.D. (In F.D.R. Form) Send Original to Tender Publishing Authority With in Time Limit
+Note:  (1) if any document file will not open, Agency has to manage to open file after downloading from N-procure site. If fail to do so, agency will be disqualified. (2) Renewal receipt of Registration and Contractor license will not be valid.</t>
   </si>
   <si>
     <t>Pre-Bid Meeting</t>
@@ -185,8 +186,8 @@
     <t>Bidding Processing Fee  ( OFFLINE)</t>
   </si>
   <si>
-    <t>900        
-												INR. (Nine hundred)</t>
+    <t>600        
+												INR. (Six hundred)</t>
   </si>
   <si>
     <t>Bidding Processing Fee Payable to</t>
@@ -205,14 +206,14 @@
 											OFFLINE)</t>
   </si>
   <si>
-    <t>6,000
-												INR. (Six thousand)</t>
+    <t>3,100
+												INR. (Three thousand One hundred)</t>
   </si>
   <si>
     <t>Bid Security/EMD/Proposal Security INR Payable to</t>
   </si>
   <si>
-    <t>Deputy Executive Engineer, Sachivalaya Complex Electrical Sub Division No 2, Gandhinagar.</t>
+    <t>Deputy Executive Engineer, Sachivalaya Complex Electrical Sub Division No 3, Gandhinagar.</t>
   </si>
   <si>
     <t>Bid Security/EMD/Proposal Security INR Payable at</t>
@@ -227,7 +228,7 @@
     <t>Officer Inviting Bids</t>
   </si>
   <si>
-    <t>Dy. Executive Engineer, Sachivalaya Complex Electrical Sub Division No 2, Gandhinagar.</t>
+    <t>DEPUTY EXECUIVE ENGINEER, S.C. ELECTRICAL SUB DN NO 3, GANDHINAGAR</t>
   </si>
   <si>
     <t>Bid Opening Authority</t>
@@ -236,13 +237,13 @@
     <t>Address</t>
   </si>
   <si>
-    <t>1st Floor A Block, Patnagar Yojna Bhavan, Sector No 16, Gandhinagar.</t>
+    <t>A BLOCK, 1ST FLOOR, PATNAGAR YOJNA BHAVAN, SECTOR NO 16, GANDHINAGAR</t>
   </si>
   <si>
     <t>Contact Details</t>
   </si>
   <si>
-    <t>07923259469</t>
+    <t>rnbele3@gmail.com</t>
   </si>
   <si>
     <t>Tender Stages</t>
@@ -341,37 +342,13 @@
     <t>kindly attach scan copy of G.S.T number or in case of Exemption attach scan copy of  C.A certificate showing annual turnover</t>
   </si>
   <si>
-    <t>Kindly attach Scan copy of E-2 and Above Category Registration [Electrical] [ Renewal Receipt of Registration is not valid]</t>
+    <t>Kindly Attach Scan Copy of E-2 and Above Category Registration [Electrical] [Renewal Receipt is Not Valid]</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>Kindly attach Scanned Copy of Valid Electrical Contractor License [ Renewal Receipt of Electrical Contractor License is no Valid]</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>The Bidder must have one office / Workshop / Service Centre in Gujarat. (Copy of documents to prove Local office / Workshop in Gujarat Please attach the copy of any one of the following: Property tax bill/Electricity Bill/Telephone Bill/GST Registration copy/Lease agreement etc.)</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Upload scan copy of Declaration Letter of Bidder As per Annexure-A</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Upload scan copy of Form-3A issued by employer to substantiate successful experience of similar work as prescribed in pre-qualification Criteria.(If require attach agreement copy) As per Annexure-C (Similar work definition specified in Annexure-C) . ( Attach agreement copy with 3A for similar type Work)</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Bidder should have Annual financial turnover of Rs. 533300.00 &amp; more during the last 5 (five) financial years from current financial year,. The C.A. Audited Certificate of Annual Turnover for the last five financial year to be Submitted. During any one of the last five financial years, ending 31st March 2025 (Certificate of Chartered Accountant or other suitable documents to the satisfaction of Tender inviting Authority).</t>
+    <t>Kindly attach scan copy of Valid Electrical Contractor Licence [Renewal Receipt is Not Valid]</t>
   </si>
   <si>
     <t>2. Commercial Stage</t>
@@ -389,13 +366,13 @@
     <t>Cert Serial No.</t>
   </si>
   <si>
-    <t>62493aeb</t>
+    <t>624b38f0</t>
   </si>
   <si>
     <t>Subject Dn</t>
   </si>
   <si>
-    <t>CN=SHAILESH KUMAR CHANDRABHAN YADAV, SERIALNUMBER=02f12e0cb242c0d1ba6d8692effa6c30e6549d77b561dab725d42dd9e360cf9e, ST=Gujarat, OID.2.5.4.17=382016, OU="DEPUTY EXECUTIVE ANGINEER,CID - 6950168", OID.2.5.4.20=40051c713e270bce7dde5f96a115ec4741ea11480a1d2ade09756feb326f6192, O=R AND B DEPARTMENT, C=IN</t>
+    <t>'CN=KISHORKUMAR B KHACHAR, SERIALNUMBER=4722f9dd212282439ae28b6b567bf03288ce598d6e02550b88ba1b206bb2600c, ST=Gujarat, OID.2.5.4.17=382016, OU="DEPUTY EXECUTIVE ENGINEERS,CID - 7035833", OID.2.5.4.20=990df54402f90cc20b4b21face775bcd9e427acab6a163a184db4bae175adc6a, O=S C ELECTRICAL SUB DIVISION NO 3 R AND B, C=IN'</t>
   </si>
   <si>
     <t>Cert Issuer</t>
@@ -407,7 +384,7 @@
     <t>Thumbprint</t>
   </si>
   <si>
-    <t>11 59 b6 9b fc 2f 60 e8 69 dc 8e 59 9f 8b 9a 7b 60 5d a1 6c</t>
+    <t>93 f0 92 36 81 9e 1d e1 88 44 42 69 f4 a0 23 d1 7c e5 78 db</t>
   </si>
   <si>
     <t>General Terms &amp; Conditions</t>
@@ -416,41 +393,41 @@
     <t>Document Definition</t>
   </si>
   <si>
-    <t>ANNEXURE C.pdf</t>
-  </si>
-  <si>
-    <t>ANX A.pdf</t>
+    <t>https://rnbtender.nprocure.com/common/download?uid=1c75364c-5087-4d51-ab9a-1dabccfaba4b&amp;name=G S T LTR.pdf</t>
   </si>
   <si>
     <t>G S T LTR.pdf</t>
   </si>
   <si>
+    <t>https://rnbtender.nprocure.com/common/download?uid=cab53588-2c70-469a-b3e8-0ec1535debda&amp;name=GR.pdf</t>
+  </si>
+  <si>
     <t>GR.pdf</t>
   </si>
   <si>
-    <t>MEMORANDUM OF WORKS.pdf</t>
-  </si>
-  <si>
-    <t>Nivida 5.pdf</t>
-  </si>
-  <si>
-    <t>PQ.pdf</t>
-  </si>
-  <si>
-    <t>SBD.pdf</t>
-  </si>
-  <si>
-    <t>SCHEDULE A.pdf</t>
-  </si>
-  <si>
-    <t>SCHEDULE B.pdf</t>
+    <t>https://rnbtender.nprocure.com/common/download?uid=ebdcb2ce-e760-4676-8f6c-b1715c04cca3&amp;name=NOTICE NO 05.pdf</t>
+  </si>
+  <si>
+    <t>NOTICE NO 05.pdf</t>
+  </si>
+  <si>
+    <t>https://rnbtender.nprocure.com/common/download?uid=3fc51b92-d593-4b04-a8c5-245cdf0d3ca5&amp;name=SBD Document.pdf</t>
+  </si>
+  <si>
+    <t>SBD Document.pdf</t>
+  </si>
+  <si>
+    <t>https://rnbtender.nprocure.com/common/download?uid=ee73d664-95db-41be-840d-934c71091a82&amp;name=schedule a b and c.pdf</t>
+  </si>
+  <si>
+    <t>schedule a b and c.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +439,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,14 +466,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -789,19 +784,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.81640625" customWidth="1"/>
-    <col min="2" max="2" width="37.90625" customWidth="1"/>
-    <col min="3" max="3" width="34.08984375" customWidth="1"/>
-    <col min="4" max="4" width="23.08984375" customWidth="1"/>
-    <col min="5" max="5" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="67" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.453125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -814,170 +809,170 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -991,66 +986,66 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1064,58 +1059,58 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1129,34 +1124,34 @@
       <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1181,24 +1176,24 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1229,36 +1224,36 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1283,341 +1278,246 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C63" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C64" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B67" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C65" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+      <c r="B68" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B68" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68" t="s">
-        <v>118</v>
-      </c>
-      <c r="D68" t="s">
-        <v>28</v>
-      </c>
-      <c r="E68" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>120</v>
-      </c>
-      <c r="B70" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>124</v>
-      </c>
-      <c r="B72" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>126</v>
-      </c>
-      <c r="B73" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
+      <c r="B75" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>96</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="A76" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C76" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>98</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="C76" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C77" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>100</v>
-      </c>
-      <c r="B78" t="s">
-        <v>132</v>
-      </c>
-      <c r="C78" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>102</v>
-      </c>
-      <c r="B79" t="s">
-        <v>133</v>
-      </c>
-      <c r="C79" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>88</v>
-      </c>
-      <c r="B80" t="s">
-        <v>134</v>
-      </c>
-      <c r="C80" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" t="s">
-        <v>135</v>
-      </c>
-      <c r="C81" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>106</v>
-      </c>
-      <c r="B82" t="s">
-        <v>136</v>
-      </c>
-      <c r="C82" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>108</v>
-      </c>
-      <c r="B83" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>110</v>
-      </c>
-      <c r="B84" t="s">
-        <v>138</v>
-      </c>
-      <c r="C84" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>112</v>
-      </c>
-      <c r="B85" t="s">
-        <v>139</v>
-      </c>
-      <c r="C85" t="s">
-        <v>139</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B72" r:id="rId1" xr:uid="{E5E7DBBD-4FE9-4D89-B945-932065A2C301}"/>
+    <hyperlink ref="B75" r:id="rId2" xr:uid="{CCE1C5F1-25D3-4E5C-9C9C-FD32B9C03807}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
extracting all the table data from details page.
</commit_message>
<xml_diff>
--- a/all_tables.xlsx
+++ b/all_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Backup\Web Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CD264D-2377-494F-A7AA-482BB72335D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C8510D-F34E-4244-8D01-7626F4614A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="132">
-  <si>
-    <t>Tender ID- 200717View BOQ/Item Details</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="136">
+  <si>
+    <t>Tender ID- 200751View BOQ/Item Details</t>
   </si>
   <si>
     <t>Organization Name</t>
@@ -34,7 +34,7 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Gandhinagar</t>
+    <t>Tapi</t>
   </si>
   <si>
     <t>Department</t>
@@ -43,13 +43,13 @@
     <t>Sub Department</t>
   </si>
   <si>
-    <t>S.C. Electrical Sub Division No. 3</t>
+    <t>Panchayat Division Tapi</t>
   </si>
   <si>
     <t>IFB/Tender Notice No</t>
   </si>
   <si>
-    <t>05/04 OF 2025/2026</t>
+    <t>06 OF 2025-26</t>
   </si>
   <si>
     <t>Tender Type</t>
@@ -61,7 +61,7 @@
     <t>Tender title/Name Of Project</t>
   </si>
   <si>
-    <t>PROVIDING STREET LIGHT POLES AT VARIOUS PLACES UNDER STREET LIGHT SECTION,GANDHINAGAR</t>
+    <t>MMGSY 2025-56  Const. of Various Box Culvert Work in Uchchhal Taluka Package No.5 Total 2 Box Culvert [1] Box Culvert in Bhadbhunja Village Jehari nagar faliya Ch 0/6 to 0/80 [2] Box Culvert in Katasvan Village Near Dudh dairy Ch 1/6 to 1/80 Ta.Uchchhal.</t>
   </si>
   <si>
     <t>Description of Material/Name of Work</t>
@@ -82,7 +82,7 @@
     <t>Product Category</t>
   </si>
   <si>
-    <t>Electrical</t>
+    <t>Civil Works - Bridges</t>
   </si>
   <si>
     <t>Tender Category</t>
@@ -94,7 +94,7 @@
     <t>Estimated Cost Value</t>
   </si>
   <si>
-    <t>306982.43 INR.  (Three lacs Zero Six Thousand Nine hundred Eighty Two Point Four  Three Only)</t>
+    <t>13106221.39 INR.  (One crore Thirty One Lacs Zero Six Thousand Two hundred Twenty One Point Three  Nine Only)</t>
   </si>
   <si>
     <t>Is ECV Visible to Supplier?</t>
@@ -118,7 +118,7 @@
     <t>Period of Completion/Delivery Period</t>
   </si>
   <si>
-    <t>20  Days</t>
+    <t>9  Months</t>
   </si>
   <si>
     <t>Procurement Type</t>
@@ -142,13 +142,13 @@
     <t>Bid Document Download Start Date</t>
   </si>
   <si>
-    <t>02-07-2025 12:15</t>
+    <t>02-07-2025 14:30</t>
   </si>
   <si>
     <t>Bid document download End Date</t>
   </si>
   <si>
-    <t>14-07-2025 16:00</t>
+    <t>16-07-2025 18:00</t>
   </si>
   <si>
     <t>Bid Submission Start Date</t>
@@ -163,8 +163,8 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Demand Draft Tender fee and E.M.D. in FDR form (not Less than 180 days) / Demand Drfat / Exemption Certificate shall be submitted in electronic format only through online (by scanning) while uploading the bid. This submission shall mean that E.M.D. &amp; tender fee are received for purpose of opening the bid. Accordingly offer of those shall be opened whose E.M.D. and tender fee is received electronically. However for the purpose of realization of D.D. bidder shall send the D.D. in original through R.P.A.D. so as to reach to Dy. Executive Engineer, Sachivalaya Complex Electrical Sub Division No. 3, Gandhinagar within 7 days from the date of tender Opening. Penaltative action for not submitting D.D. in original to Executive Engineer by bidder shall be initiated. D.D. for Exemption Certificate is not necessary. However Exemption Certificate shall have to be submitted electronically through online. If the contractor does not remit the tender fee &amp; the earnest money within the specified time his registration will be held in abeyance for one year &amp; his tendering code will be cancelled for one year. Any documents in supporting of tender bid shall be submitted in electronic format only through online (by scanning etc.) and hard copy will not be accepted separately. (R. &amp; B. Circular No: PRC-102008-5-S, dated 18-01-2008 &amp; R. &amp; B. D.G.R.No: Parach-102008-5-C (Partfile), dated 27-11-2008). Note:- Only Tender Fee and E.M.D. (In F.D.R. Form) Send Original to Tender Publishing Authority With in Time Limit
-Note:  (1) if any document file will not open, Agency has to manage to open file after downloading from N-procure site. If fail to do so, agency will be disqualified. (2) Renewal receipt of Registration and Contractor license will not be valid.</t>
+    <t>Demand draft for Tender Fee &amp; EMD for FDR shall be submitted in electronic format only through online (by scanning) while uploading the bid. This submission shall mean that E.M.D. &amp; tender fee are received for purpose of opening the bid. Accordingly offer of those shall be opened whose E.M.D. &amp; tender fee is received electronically. However for the purpose of realization of D.D., bidder shall send the D.D. in  riginal through R.P.A.D. so as to reach to S.E. at the time of tender opening or send the same through R.P.A.D. so as to reach to Executive Engineer, Panchayat (R&amp;B) Division, Tapi., Vyara within 7 days from  he last date of Uploding. Penaltative action for not submitting D.D. in original to E.E. by bidder shall be  nitiated and action shall be taken for abeyance of registration and cancellation of E-Tendering code for a period of one year as Govt. Circular Dt. 27/11/2008. F.D.R. for exemption Certificate is not necessary. D.D. for Exemption Certificate is not necessary. However Exemption Certificate shall have to be submitted electronically through online. (By scanning) Eligibility- Registration Certificate of Approved Class -“C” Class 
+Special Cat-III (Bridge and Above) Any documents in supporting of bid shall be submitted in electronic format only through online (by scanning) &amp; hard copy will not be accepted separately. Valid Bank Solvency issued on or after 1/1/2025.</t>
   </si>
   <si>
     <t>Pre-Bid Meeting</t>
@@ -186,64 +186,73 @@
     <t>Bidding Processing Fee  ( OFFLINE)</t>
   </si>
   <si>
-    <t>600        
-												INR. (Six hundred)</t>
+    <t>3,600        
+												INR. (Three thousand Six hundred)</t>
   </si>
   <si>
     <t>Bidding Processing Fee Payable to</t>
   </si>
   <si>
-    <t>Executive Engineer, Sachivalaya Complex Electrical Division, Gandhinagar.</t>
+    <t>Executive Engineer, Panchayat (R&amp;B) Division, Tapi-Vyara</t>
   </si>
   <si>
     <t>Bidding Processing Fee Payable at</t>
   </si>
   <si>
-    <t>GANDHINAGAR</t>
+    <t>Vyara</t>
   </si>
   <si>
     <t>Bid Security/EMD/Proposal Security INR (
 											OFFLINE)</t>
   </si>
   <si>
-    <t>3,100
-												INR. (Three thousand One hundred)</t>
+    <t>132,000
+												INR. (One lac Thirty Two Thousand)</t>
   </si>
   <si>
     <t>Bid Security/EMD/Proposal Security INR Payable to</t>
   </si>
   <si>
-    <t>Deputy Executive Engineer, Sachivalaya Complex Electrical Sub Division No 3, Gandhinagar.</t>
-  </si>
-  <si>
     <t>Bid Security/EMD/Proposal Security INR Payable at</t>
   </si>
   <si>
     <t>Exempted Fee</t>
   </si>
   <si>
+    <t>Minimum FDR</t>
+  </si>
+  <si>
+    <t>132,000 INR.</t>
+  </si>
+  <si>
+    <t>Maximum FDR</t>
+  </si>
+  <si>
     <t>Other Details</t>
   </si>
   <si>
     <t>Officer Inviting Bids</t>
   </si>
   <si>
-    <t>DEPUTY EXECUIVE ENGINEER, S.C. ELECTRICAL SUB DN NO 3, GANDHINAGAR</t>
+    <t>Executive Engineer, Panchayat (R&amp;B) Division, Tapi</t>
   </si>
   <si>
     <t>Bid Opening Authority</t>
   </si>
   <si>
+    <t>Superintending Engineer, Panchayat (R&amp;B) Circle, Surat</t>
+  </si>
+  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>A BLOCK, 1ST FLOOR, PATNAGAR YOJNA BHAVAN, SECTOR NO 16, GANDHINAGAR</t>
+    <t>Nanpura, Dutch Garden, Surat</t>
   </si>
   <si>
     <t>Contact Details</t>
   </si>
   <si>
-    <t>rnbele3@gmail.com</t>
+    <t>2626220081</t>
   </si>
   <si>
     <t>Tender Stages</t>
@@ -261,7 +270,7 @@
     <t>Preliminary Stage</t>
   </si>
   <si>
-    <t>14-07-2025 16:05</t>
+    <t>17-07-2025 11:05</t>
   </si>
   <si>
     <t>0</t>
@@ -270,7 +279,7 @@
     <t>Commercial Stage</t>
   </si>
   <si>
-    <t>14-07-2025 16:10</t>
+    <t>17-07-2025 11:10</t>
   </si>
   <si>
     <t>1. Preliminary Stage</t>
@@ -318,37 +327,46 @@
     <t>1</t>
   </si>
   <si>
-    <t>Kindly attach Scan copy of Tender fee</t>
+    <t>Attached Copy of Tender Fee</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>Kindly attach Scan copy of E.M.D. in FDR Form (Not Less than 180 Days) / Exemption certificate</t>
+    <t>Attached Copy of EMD</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Kindly attach Scan copy of Current Calendar Year Bank Solvency of 20 Percentage Amount put to tender of Nationalized / Schedule Bank  2025</t>
+    <t>Attached Copy of Registration of Class</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>Kindly attach Scan copy of PAN Card etc</t>
-  </si>
-  <si>
-    <t>kindly attach scan copy of G.S.T number or in case of Exemption attach scan copy of  C.A certificate showing annual turnover</t>
-  </si>
-  <si>
-    <t>Kindly Attach Scan Copy of E-2 and Above Category Registration [Electrical] [Renewal Receipt is Not Valid]</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Kindly attach scan copy of Valid Electrical Contractor Licence [Renewal Receipt is Not Valid]</t>
+    <t>Attached Copy of Pan Card &amp; GST Registration</t>
+  </si>
+  <si>
+    <t>Attached Copy of Valid Bank Solvency Certificate for Calendar year 2025</t>
+  </si>
+  <si>
+    <t>Attached Copy of all Required Documents as per Tender Condition</t>
+  </si>
+  <si>
+    <t>Documents required For Form - Tender Fee Form</t>
+  </si>
+  <si>
+    <t>Provide any proof of Bid Processing Fee</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Documents required For Form - Emd Fee Form</t>
+  </si>
+  <si>
+    <t>Provide any proof of EMD Document</t>
   </si>
   <si>
     <t>2. Commercial Stage</t>
@@ -366,13 +384,13 @@
     <t>Cert Serial No.</t>
   </si>
   <si>
-    <t>624b38f0</t>
+    <t>624b0e7b</t>
   </si>
   <si>
     <t>Subject Dn</t>
   </si>
   <si>
-    <t>'CN=KISHORKUMAR B KHACHAR, SERIALNUMBER=4722f9dd212282439ae28b6b567bf03288ce598d6e02550b88ba1b206bb2600c, ST=Gujarat, OID.2.5.4.17=382016, OU="DEPUTY EXECUTIVE ENGINEERS,CID - 7035833", OID.2.5.4.20=990df54402f90cc20b4b21face775bcd9e427acab6a163a184db4bae175adc6a, O=S C ELECTRICAL SUB DIVISION NO 3 R AND B, C=IN'</t>
+    <t>CN=DHARMESH A PATEL, SERIALNUMBER=63b1ac1c22dfb9428fb6326ad56abf34794fe0fe2d315b1c6bbb5aa33f5d4059, ST=Gujarat, OID.2.5.4.17=394652, OU="ROAD AND BUILDING,CID - 7028566", OID.2.5.4.20=7cff5a3a4de6dd80b359494213d267466d10507dc699febdb47a8c28bf7606bf, O=OFFICE OF EXECUTIVE ENGINEER PANCHAYAT R AND B DIVISION, C=IN</t>
   </si>
   <si>
     <t>Cert Issuer</t>
@@ -384,7 +402,7 @@
     <t>Thumbprint</t>
   </si>
   <si>
-    <t>93 f0 92 36 81 9e 1d e1 88 44 42 69 f4 a0 23 d1 7c e5 78 db</t>
+    <t>46 91 7b b2 21 46 dc 19 c4 1e 6d 6c e4 ca bc 94 72 5e 71 3e</t>
   </si>
   <si>
     <t>General Terms &amp; Conditions</t>
@@ -393,41 +411,35 @@
     <t>Document Definition</t>
   </si>
   <si>
-    <t>https://rnbtender.nprocure.com/common/download?uid=1c75364c-5087-4d51-ab9a-1dabccfaba4b&amp;name=G S T LTR.pdf</t>
-  </si>
-  <si>
-    <t>G S T LTR.pdf</t>
-  </si>
-  <si>
-    <t>https://rnbtender.nprocure.com/common/download?uid=cab53588-2c70-469a-b3e8-0ec1535debda&amp;name=GR.pdf</t>
+    <t>https://rnbtender.nprocure.com/common/download?uid=c53ea967-bde2-4e14-8863-d5b360dbcf84&amp;name=SBD_Pkg-5 Uchchhal 2 Box Culvert.pdf</t>
+  </si>
+  <si>
+    <t>SBD_Pkg-5 Uchchhal 2 Box Culvert.pdf</t>
+  </si>
+  <si>
+    <t>https://rnbtender.nprocure.com/common/download?uid=bce87e00-8fa6-49b6-8347-cdc551f64720&amp;name=BOQ_Pkg-5 Uchchhal 2 Box Culvert.pdf</t>
+  </si>
+  <si>
+    <t>BOQ_Pkg-5 Uchchhal 2 Box Culvert.pdf</t>
+  </si>
+  <si>
+    <t>https://rnbtender.nprocure.com/common/download?uid=df62bec4-a01d-4279-be02-be48b4ee3805&amp;name=Specification _Pkg-5 Uchchhal 2 Box Culvert.pdf</t>
+  </si>
+  <si>
+    <t>Specification _Pkg-5 Uchchhal 2 Box Culvert.pdf</t>
+  </si>
+  <si>
+    <t>https://rnbtender.nprocure.com/common/download?uid=1a8ddd9a-243d-4a23-919b-8e3cf65ccbce&amp;name=GR.pdf</t>
   </si>
   <si>
     <t>GR.pdf</t>
-  </si>
-  <si>
-    <t>https://rnbtender.nprocure.com/common/download?uid=ebdcb2ce-e760-4676-8f6c-b1715c04cca3&amp;name=NOTICE NO 05.pdf</t>
-  </si>
-  <si>
-    <t>NOTICE NO 05.pdf</t>
-  </si>
-  <si>
-    <t>https://rnbtender.nprocure.com/common/download?uid=3fc51b92-d593-4b04-a8c5-245cdf0d3ca5&amp;name=SBD Document.pdf</t>
-  </si>
-  <si>
-    <t>SBD Document.pdf</t>
-  </si>
-  <si>
-    <t>https://rnbtender.nprocure.com/common/download?uid=ee73d664-95db-41be-840d-934c71091a82&amp;name=schedule a b and c.pdf</t>
-  </si>
-  <si>
-    <t>schedule a b and c.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,14 +451,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -466,24 +470,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -784,19 +778,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="67" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="38.1796875" customWidth="1"/>
+    <col min="2" max="2" width="56.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -809,170 +800,170 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -986,66 +977,66 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1059,465 +1050,517 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+      <c r="A34" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="2" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E51" s="2" t="s">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>91</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="B61" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="B62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C64" s="2" t="s">
+      <c r="A64" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" t="s">
         <v>110</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
+      <c r="C65" t="s">
         <v>111</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>99</v>
+      </c>
+      <c r="B68" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
+      <c r="C68" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" t="s">
+        <v>116</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="B74" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B72" s="3" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="B75" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>124</v>
+      </c>
+      <c r="B76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B75" s="3" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>99</v>
+      </c>
+      <c r="B79" t="s">
         <v>128</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C79" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B76" s="2" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>101</v>
+      </c>
+      <c r="B80" t="s">
         <v>130</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C80" t="s">
         <v>131</v>
       </c>
     </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>103</v>
+      </c>
+      <c r="B81" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82" t="s">
+        <v>134</v>
+      </c>
+      <c r="C82" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B72" r:id="rId1" xr:uid="{E5E7DBBD-4FE9-4D89-B945-932065A2C301}"/>
-    <hyperlink ref="B75" r:id="rId2" xr:uid="{CCE1C5F1-25D3-4E5C-9C9C-FD32B9C03807}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>